<commit_message>
A Dog Said... Animal Prosthetics 2 업데이트
</commit_message>
<xml_diff>
--- a/Pull Request Here/A Dog Said 2 - 3238353862/A Dog Said... Animal Prosthetics 2 - 3238353862.xlsx
+++ b/Pull Request Here/A Dog Said 2 - 3238353862/A Dog Said... Animal Prosthetics 2 - 3238353862.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93F785D-7A45-4ED6-9C2C-AA23625D76F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99357685-40EF-47D1-99AF-99C97C8B8661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5557,10 +5557,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>동물 날개 보철물입니다. 신경 연결 요소가 부족하지만, 내부 관절과 날개 막의 정밀한 배열 덕분에 자연스러운 움직임이 가능합니다. 그렇지만 실제 동물 날개보다는 못합니다. 날개가 필요한 이식 가능합니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>진보된 인공 동물 날개입니다. 바이오젤 신경 연결기, 가벼운 합성막, 미세 격자 치유 시스템 등 모든 면에서 생물학적 날개보다 월등합니다. 날개가 필요한 동물에게 이식 가능합니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -5586,6 +5582,10 @@
   </si>
   <si>
     <t>이식된 나무 날개입니다. 어설프지만 다시 날 수 있습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>동물 날개 보철물입니다. 신경 연결 요소가 부족하지만, 내부 관절과 날개 막의 정밀한 배열 덕분에 자연스러운 움직임이 가능합니다. 그렇지만 실제 동물 날개보다는 못합니다. 날개가 필요한 동물에게 이식 가능합니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -7725,7 +7725,7 @@
         <v>1352</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -14459,7 +14459,7 @@
         <v>1420</v>
       </c>
       <c r="F437" s="6" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.3">
@@ -14479,7 +14479,7 @@
         <v>1419</v>
       </c>
       <c r="F438" s="6" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.3">
@@ -14499,7 +14499,7 @@
         <v>1423</v>
       </c>
       <c r="F439" s="6" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.3">
@@ -14519,7 +14519,7 @@
         <v>1061</v>
       </c>
       <c r="F440" s="6" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.3">
@@ -14539,7 +14539,7 @@
         <v>1064</v>
       </c>
       <c r="F441" s="6" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.3">
@@ -14559,7 +14559,7 @@
         <v>1067</v>
       </c>
       <c r="F442" s="6" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.3">
@@ -14659,7 +14659,7 @@
         <v>1425</v>
       </c>
       <c r="F447" s="6" t="s">
-        <v>1680</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="448" spans="1:6" x14ac:dyDescent="0.3">
@@ -14819,7 +14819,7 @@
         <v>1097</v>
       </c>
       <c r="F455" s="6" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>